<commit_message>
update demandes de stage + nouvelles demandes
</commit_message>
<xml_diff>
--- a/Stage/récap contact stage.xlsx
+++ b/Stage/récap contact stage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="59">
   <si>
     <t xml:space="preserve">Entreprise</t>
   </si>
@@ -161,6 +161,42 @@
   </si>
   <si>
     <t xml:space="preserve">https://fr.indeed.com/voir-emploi?cmp=Nelis&amp;t=Stagiaire+D%C3%A9veloppeur+Web&amp;jk=db89470ac3bab56c&amp;q=Stage+D%C3%A9veloppeur+Web&amp;vjs=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eureka Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.eureka-technology.fr/fr-fr/contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyce Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.indeed.com/voir-emploi?jk=d4301b224a275145&amp;hl=fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximilien GARENNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximilien.garenne@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sidy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact@sidy.fr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enzo VIRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enzo.viry@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lundi Matin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://fr.indeed.com/voir-emploi?cmp=LUNDI-MATIN&amp;t=Stagiaire+D%C3%A9veloppeur+Web&amp;jk=df33a59f13bbcd97&amp;q=Stage+D%C3%A9veloppeur+Web&amp;vjs=3</t>
   </si>
 </sst>
 </file>
@@ -171,7 +207,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -219,11 +255,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -280,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -314,10 +345,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -405,10 +432,10 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -514,7 +541,7 @@
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7" t="n">
-        <v>44439</v>
+        <v>44468</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="6"/>
@@ -616,14 +643,16 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7" t="n">
-        <v>44454</v>
+        <v>44466</v>
       </c>
       <c r="H10" s="7"/>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="J10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,7 +683,7 @@
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="7" t="n">
-        <v>44439</v>
+        <v>44468</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="6"/>
@@ -773,10 +802,10 @@
         <v>8</v>
       </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="10" t="n">
+      <c r="G18" s="9" t="n">
         <v>44460</v>
       </c>
-      <c r="H18" s="10"/>
+      <c r="H18" s="9"/>
       <c r="I18" s="6" t="s">
         <v>9</v>
       </c>
@@ -792,14 +821,16 @@
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F19" s="6"/>
-      <c r="G19" s="10" t="n">
-        <v>44466</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="9" t="n">
+        <v>44467</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="J19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,82 +846,130 @@
         <v>12</v>
       </c>
       <c r="F20" s="6"/>
-      <c r="G20" s="10" t="n">
+      <c r="G20" s="9" t="n">
         <v>44466</v>
       </c>
-      <c r="H20" s="10"/>
+      <c r="H20" s="9"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="B21" s="4"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="C21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="G21" s="9" t="n">
+        <v>44468</v>
+      </c>
+      <c r="H21" s="9"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="B22" s="4"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="C22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="G22" s="9" t="n">
+        <v>44468</v>
+      </c>
+      <c r="H22" s="9"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="C23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="G23" s="9" t="n">
+        <v>44468</v>
+      </c>
+      <c r="H23" s="9"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="C24" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="G24" s="9" t="n">
+        <v>44468</v>
+      </c>
+      <c r="H24" s="9"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4"/>
+      <c r="A25" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="C25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
+      <c r="G25" s="9" t="n">
+        <v>44468</v>
+      </c>
+      <c r="H25" s="9"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
+      <c r="A26" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
+      <c r="G26" s="9" t="n">
+        <v>44468</v>
+      </c>
+      <c r="H26" s="9"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
@@ -1130,6 +1209,12 @@
     <hyperlink ref="C17" r:id="rId13" display="https://www.arpa3.fr/agence/contact/"/>
     <hyperlink ref="C19" r:id="rId14" display="https://www.ino.global/contact/"/>
     <hyperlink ref="C20" r:id="rId15" display="https://fr.indeed.com/voir-emploi?cmp=Nelis&amp;t=Stagiaire+D%C3%A9veloppeur+Web&amp;jk=db89470ac3bab56c&amp;q=Stage+D%C3%A9veloppeur+Web&amp;vjs=3"/>
+    <hyperlink ref="C21" r:id="rId16" display="https://www.eureka-technology.fr/fr-fr/contact"/>
+    <hyperlink ref="C22" r:id="rId17" display="https://fr.indeed.com/voir-emploi?jk=d4301b224a275145&amp;hl=fr"/>
+    <hyperlink ref="C23" r:id="rId18" display="maximilien.garenne@gmail.com"/>
+    <hyperlink ref="C24" r:id="rId19" display="contact@sidy.fr"/>
+    <hyperlink ref="C25" r:id="rId20" display="enzo.viry@gmail.com"/>
+    <hyperlink ref="C26" r:id="rId21" display="https://fr.indeed.com/voir-emploi?cmp=LUNDI-MATIN&amp;t=Stagiaire+D%C3%A9veloppeur+Web&amp;jk=df33a59f13bbcd97&amp;q=Stage+D%C3%A9veloppeur+Web&amp;vjs=3"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>